<commit_message>
promene posle 1. casa predavanja
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DC833E-F3EB-4830-9C16-645894482A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10518" yWindow="7937" windowWidth="16589" windowHeight="8583" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10524" yWindow="7932" windowWidth="16584" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>Opis</t>
   </si>
@@ -53,28 +52,34 @@
     <t>Funkcionalni</t>
   </si>
   <si>
-    <t>Neophodno je da napravimo serijsku,  sekvencijalnu datoteku I tabela relacionih baza MySql. Za trajno cuvanje informacionih resursa.</t>
-  </si>
-  <si>
-    <t>Neophodno je da omogucimo dodavanje novog korisnika.</t>
-  </si>
-  <si>
-    <t>Neophodno je da napravimo  profil sa podacima ulogovanog korisnika sa mogucnoscu promene podataka.</t>
-  </si>
-  <si>
-    <t>Neophodno je da napravimo kolekciju korisnika I kolekcije sa podacima o njima</t>
-  </si>
-  <si>
     <t>Neophodno je da napravimo interaktivnu pocetnu stranu sa svim alatima za upravljanje sistemom I rukovanje sa greskama.</t>
   </si>
   <si>
-    <t>Neophodno je da napravimo  obrazac za prijavljivanje korisnika I rukovanjem pravima pristupa.</t>
+    <t>1.2 da ga sacuvamo, promenimo ime, obrisemo.</t>
+  </si>
+  <si>
+    <t>Neophodno je obezbediti rukovanje informacionim resursima. Pod informacionim resursom se podrazumeva kolekcije svojstava objekata posmatranja sa cime ce se manipulisati.</t>
+  </si>
+  <si>
+    <t>1.1 inf res treba da ga kreiramo, izmenimo,  sacuvamo.</t>
+  </si>
+  <si>
+    <t>Neophodno je omoguciti dodavanje novog korisnika.</t>
+  </si>
+  <si>
+    <t>Neophodno je napraviti  obrazac za prijavljivanje korisnika I rukovanjem pravima pristupa.</t>
+  </si>
+  <si>
+    <t>Neophodno je napraviti kolekciju korisnika I kolekcije sa podacima o njima.</t>
+  </si>
+  <si>
+    <t>Neophodno je napraviti  profil sa podacima ulogovanog korisnika sa mogucnoscu promene podataka.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,23 +288,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -335,23 +323,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -527,24 +498,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.796875" defaultRowHeight="50" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="49.95" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.69921875" style="7" customWidth="1"/>
-    <col min="2" max="3" width="15.796875" style="1"/>
+    <col min="1" max="1" width="36.6640625" style="7" customWidth="1"/>
+    <col min="2" max="3" width="15.77734375" style="1"/>
     <col min="4" max="4" width="22" style="1" customWidth="1"/>
-    <col min="5" max="6" width="15.796875" style="1"/>
-    <col min="7" max="7" width="15.796875" style="2"/>
-    <col min="8" max="16384" width="15.796875" style="3"/>
+    <col min="5" max="6" width="15.77734375" style="1"/>
+    <col min="7" max="7" width="15.77734375" style="2"/>
+    <col min="8" max="16384" width="15.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="50" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="49.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -567,9 +538,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="73.900000000000006" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="94.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -590,55 +561,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="50" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" ht="73.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="83.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:7" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
@@ -656,10 +591,10 @@
         <v>9</v>
       </c>
       <c r="G5" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="69" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="49.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
@@ -679,12 +614,12 @@
         <v>9</v>
       </c>
       <c r="G6" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="57.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="83.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -702,11 +637,57 @@
         <v>9</v>
       </c>
       <c r="G7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="69" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="57.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>